<commit_message>
Forecast of last value of base 2000 GDP via an ARIMA(2,1,2) model.
</commit_message>
<xml_diff>
--- a/Belize_Quarterly.xlsx
+++ b/Belize_Quarterly.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maico\OneDrive - Universidad Nacional de Colombia\Oliver Pardo\VAR_VEC-2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/msramirezgo_unal_edu_co/Documents/Oliver Pardo/VAR_VEC-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B4C8CF-AEA0-4B62-A81C-9AB9D2DABA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{66B4C8CF-AEA0-4B62-A81C-9AB9D2DABA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F32D13AA-E1F4-4231-AA2E-BCDEDA246AF4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,7 +357,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0_);\(#,##0.0\)"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="172" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -471,10 +471,10 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -763,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4952,7 +4952,9 @@
         <f t="shared" si="7"/>
         <v>402.57170547047889</v>
       </c>
-      <c r="J91" s="3"/>
+      <c r="J91" s="3">
+        <v>741.43889999999999</v>
+      </c>
       <c r="K91" s="3">
         <v>1313.1</v>
       </c>

</xml_diff>